<commit_message>
Added dummy topics and relationships too (to test initial API + interface);
</commit_message>
<xml_diff>
--- a/server/sampleData/SampleArticles.xlsx
+++ b/server/sampleData/SampleArticles.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12100" yWindow="-640" windowWidth="12800" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Articles" sheetId="1" r:id="rId1"/>
+    <sheet name="Topics" sheetId="2" r:id="rId2"/>
+    <sheet name="Articles_Topics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,10 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Title</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Link</t>
   </si>
@@ -40,16 +39,74 @@
   </si>
   <si>
     <t>http://www.herald-dispatch.com/news/mu-neurology-s-art-auction-part-of-comprehensive-approach/article_7ced5b49-ba53-56ac-a8a6-32a26f0fbe20.html</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Article ID</t>
+  </si>
+  <si>
+    <t>Topic ID</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Neurology</t>
+  </si>
+  <si>
+    <t>Cardiology</t>
+  </si>
+  <si>
+    <t>Neurology professor mentioned</t>
+  </si>
+  <si>
+    <t>Marshall University Neurology department mentioned</t>
+  </si>
+  <si>
+    <t>http://www.mansfieldnewsjournal.com/story/news/local/2016/04/02/regions-hospitals-working-recruit-new-doctors/82511806/</t>
+  </si>
+  <si>
+    <t>Region’s hospitals working to recruit new doctors</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Neurology physicians mentioned</t>
+  </si>
+  <si>
+    <t>Cardiology physicians mentioned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,14 +129,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -409,45 +490,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>42459</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>42460</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
       <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="C2" s="1">
-        <v>42459</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1">
-        <v>42460</v>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>